<commit_message>
code of rashida is restructured
</commit_message>
<xml_diff>
--- a/resources/download/files/topup/sample_topup.xlsx
+++ b/resources/download/files/topup/sample_topup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Number</t>
   </si>
@@ -24,13 +24,10 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>topupOperatorId</t>
+    <t>01723598606</t>
   </si>
   <si>
     <t>topupType</t>
-  </si>
-  <si>
-    <t>01723598606</t>
   </si>
 </sst>
 </file>
@@ -363,24 +360,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,29 +381,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2">
-        <v>101</v>
-      </c>
-      <c r="D2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>